<commit_message>
added the pollen category viewer
</commit_message>
<xml_diff>
--- a/exampleData.xlsx
+++ b/exampleData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Google Drive\ID2050 personal\PollenTool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobys\Google Drive\ID2050 personal\Desktop\PollenTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBDE35E-526E-4475-AEBF-4973B6D9C145}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204435C1-A35D-4D87-937A-79256332C8C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9650" yWindow="980" windowWidth="9240" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,15 +414,15 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -439,13 +439,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
       <c r="D2">
         <v>100</v>
       </c>
@@ -453,7 +450,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -467,21 +464,13 @@
         <v>320</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>500</v>
-      </c>
-      <c r="D4">
-        <v>500</v>
-      </c>
-      <c r="E4" s="1">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -495,7 +484,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6"/>
     </row>
   </sheetData>

</xml_diff>